<commit_message>
permite hacer X cantidad de preguntas
</commit_message>
<xml_diff>
--- a/resources/temporary_excel.xlsx
+++ b/resources/temporary_excel.xlsx
@@ -1,41 +1,151 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Documents\Pili\IronHack\CodeQuestAPI\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7480" windowHeight="2370"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+  <si>
+    <t>Quiz template</t>
+  </si>
+  <si>
+    <t>Add questions, at least two answer alternatives, time limit and choose correct answers (at least one). Have fun creating your awesome quiz!</t>
+  </si>
+  <si>
+    <t>Remember: questions have a limit of 120 characters and answers can have 75 characters max. Text will turn red in Excel or Google Docs if you exceed this limit. If several answers are correct, separate them with a comma.</t>
+  </si>
+  <si>
+    <t>See an example question below (don't forget to overwrite this with your first question!)</t>
+  </si>
+  <si>
+    <t>And remember,  if you're not using Excel you need to export to .xlsx format before you upload to Kahoot!</t>
+  </si>
+  <si>
+    <t>Question - max 120 characters</t>
+  </si>
+  <si>
+    <t>Answer 1 - max 75 characters</t>
+  </si>
+  <si>
+    <t>Answer 2 - max 75 characters</t>
+  </si>
+  <si>
+    <t>Answer 3 - max 75 characters</t>
+  </si>
+  <si>
+    <t>Answer 4 - max 75 characters</t>
+  </si>
+  <si>
+    <t>Time limit (sec) – 5, 10, 20, 30, 60, 90, 120, or 240 secs</t>
+  </si>
+  <si>
+    <t>Correct answer(s) - choose at least one</t>
+  </si>
+  <si>
+    <t>rfedq</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>fedas</t>
+  </si>
+  <si>
+    <t>ddwas</t>
+  </si>
+  <si>
+    <t>wdwd</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>What is the default port number for HTTP?</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>443</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Which of the following is not a JavaScript data type?</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>What is the output of 0.1 + 0.2 in JavaScript?</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.30000000000000004</t>
+  </si>
+  <si>
+    <t>0.29999999999999999</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Which JavaScript keyword is used to define a constant variable?</t>
+  </si>
+  <si>
+    <t>let</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>define</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -64,7 +174,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -72,6 +183,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,577 +515,685 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1001"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H108"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="73.08203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2">
-      <c r="B2" t="str">
-        <v>Quiz template</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="str">
-        <v>Add questions, at least two answer alternatives, time limit and choose correct answers (at least one). Have fun creating your awesome quiz!</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="str">
-        <v>Remember: questions have a limit of 120 characters and answers can have 75 characters max. Text will turn red in Excel or Google Docs if you exceed this limit. If several answers are correct, separate them with a comma.</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="str">
-        <v>See an example question below (don't forget to overwrite this with your first question!)</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="str">
-        <v>And remember,  if you're not using Excel you need to export to .xlsx format before you upload to Kahoot!</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="str">
-        <v>Question - max 120 characters</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Answer 1 - max 75 characters</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Answer 2 - max 75 characters</v>
-      </c>
-      <c r="E8" t="str">
-        <v>Answer 3 - max 75 characters</v>
-      </c>
-      <c r="F8" t="str">
-        <v>Answer 4 - max 75 characters</v>
-      </c>
-      <c r="G8" t="str">
-        <v>Time limit (sec) – 5, 10, 20, 30, 60, 90, 120, or 240 secs</v>
-      </c>
-      <c r="H8" t="str">
-        <v>Correct answer(s) - choose at least one</v>
-      </c>
-    </row>
-    <row r="9">
+    <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="str">
-        <v>Which of the following is not a JavaScript data type?</v>
-      </c>
-      <c r="C9" t="str">
-        <v>String</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Boolean</v>
-      </c>
-      <c r="E9" t="str">
-        <v>Float</v>
-      </c>
-      <c r="F9" t="str">
-        <v>Object</v>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
       </c>
       <c r="G9">
         <v>30</v>
       </c>
-      <c r="H9" t="str">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>7</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>8</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>9</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>10</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>11</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>12</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>13</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>14</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>15</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>16</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>17</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>18</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>19</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>20</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>21</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>22</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>23</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>24</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>25</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>26</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>27</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>28</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>29</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>30</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>31</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>32</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>33</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>34</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>35</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>36</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>37</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>38</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>39</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>40</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>41</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>42</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>43</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>44</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>45</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>46</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>47</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>48</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>49</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>50</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>51</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>52</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>53</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>54</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>55</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>56</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>57</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>58</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>59</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>60</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>61</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>62</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>63</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>64</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>65</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>66</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>67</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>68</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>69</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>70</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>71</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>72</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>73</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>74</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>75</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>76</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>77</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>78</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>79</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>80</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>81</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>82</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>83</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>84</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>85</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>86</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>87</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>88</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>89</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>90</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>91</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>92</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>93</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>94</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>95</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>96</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>97</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>98</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>99</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>100</v>
       </c>
@@ -977,9 +1204,9 @@
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B6:H6"/>
   </mergeCells>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA1001"/>
+    <ignoredError sqref="A1:AA1001" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>